<commit_message>
Codigo de inserir a partir de excel refatorado e validando arquivos excel apenas
</commit_message>
<xml_diff>
--- a/BackEnd/Cliente/EurofarmaCliente/src/main/resources/EmployeeDocuments/Funcionarios.xlsx
+++ b/BackEnd/Cliente/EurofarmaCliente/src/main/resources/EmployeeDocuments/Funcionarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Eurofarma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63052C9F-7E7E-486F-B158-13D34FF65F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1DFC5A-D7E2-4EAF-8BCE-E06EDF92118F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{FD8F463F-932E-4A5F-B508-AA28C5DD5B04}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -90,14 +90,34 @@
   </si>
   <si>
     <t>DAS</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Malaquias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -125,8 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DEE1A9-9E85-4F5B-9A54-3C81E2BCF23B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,9 +494,11 @@
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -494,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31342</v>
       </c>
@@ -514,7 +538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13464</v>
       </c>
@@ -534,7 +558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1314</v>
       </c>
@@ -554,7 +578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>443</v>
       </c>
@@ -574,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>133</v>
       </c>
@@ -593,6 +617,170 @@
       <c r="F6" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6252</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1331241241</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3131</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3135515135</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>313</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3113513513</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>455</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2">
+        <v>33552334554657</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>6546</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2">
+        <v>562434414</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9078</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>457984664</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>875</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2">
+        <v>467425644</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>78456</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4675434355</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionado função de enviar sms com as informações do usuário para o numero cadastrado no insertAll
</commit_message>
<xml_diff>
--- a/BackEnd/Cliente/EurofarmaCliente/src/main/resources/EmployeeDocuments/Funcionarios.xlsx
+++ b/BackEnd/Cliente/EurofarmaCliente/src/main/resources/EmployeeDocuments/Funcionarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Eurofarma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1DFC5A-D7E2-4EAF-8BCE-E06EDF92118F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5B9C1F-8528-4298-826B-5BF2B211D3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2070" yWindow="3210" windowWidth="21600" windowHeight="11295" xr2:uid="{FD8F463F-932E-4A5F-B508-AA28C5DD5B04}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -102,22 +102,20 @@
   </si>
   <si>
     <t>Malaquias</t>
+  </si>
+  <si>
+    <t>Renato</t>
+  </si>
+  <si>
+    <t>Kenzo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -145,10 +143,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DEE1A9-9E85-4F5B-9A54-3C81E2BCF23B}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +494,7 @@
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -518,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>31342</v>
       </c>
@@ -538,7 +534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13464</v>
       </c>
@@ -558,7 +554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1314</v>
       </c>
@@ -578,7 +574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>443</v>
       </c>
@@ -598,7 +594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>133</v>
       </c>
@@ -618,169 +614,305 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6252</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>1331241241</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>3131</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>3135515135</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>313</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>3113513513</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>455</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>33552334554657</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>6546</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>562434414</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9078</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>457984664</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>875</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>467425644</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>78456</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>4675434355</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5124</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>5532525325</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>45543</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>41424214214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7895</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>422526236</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>46755</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>526752532</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>31465</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>21467534732</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6788</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>4414124214</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21342</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>5511999381877</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>